<commit_message>
Rename Report Message Column
Message column is now renamed to Description for clear understanding of the meaning of the data that the column stores
</commit_message>
<xml_diff>
--- a/src/Data/Config.xlsx
+++ b/src/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nicoerlichman\Documents\2-Code_Repos\UiPath\Custom-REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nicoerlichman\Documents\2-Code_Repos\UiPath\Custom-REFramework\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E808A2-F660-4560-A64F-8A1902ADD4C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573F3724-143B-4C32-BADF-3A9C93DCFF56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>MaxRetryNumber</t>
   </si>
@@ -110,18 +110,9 @@
     <t>Report_StatusColumnName</t>
   </si>
   <si>
-    <t>Report_MessageColumnName</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>Name of the column that is going to store the status of the transaction in the report</t>
   </si>
   <si>
-    <t>Name of the column that is going to store the message of the transaction in the report</t>
-  </si>
-  <si>
     <t>It indicates the email accounts (separated by semicolon) that are meant to recive the reporting email. Should be left empty if reporting email functionality isn't needed</t>
   </si>
   <si>
@@ -222,6 +213,12 @@
   </si>
   <si>
     <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
+  </si>
+  <si>
+    <t>Report_DescriptionColumnName</t>
+  </si>
+  <si>
+    <t>Name of the column that is going to store the description of the transaction error in the report</t>
   </si>
 </sst>
 </file>
@@ -746,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B9EE4A-A787-482A-9A13-E1DF8641FC90}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -757,7 +754,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -765,47 +762,47 @@
     </row>
     <row r="3" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -813,32 +810,32 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -866,13 +863,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1898,13 +1895,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2925,13 +2922,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2944,8 +2941,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2958,13 +2955,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3004,24 +3001,24 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5" s="17">
         <v>0</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3151,13 +3148,13 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3168,29 +3165,29 @@
         <v>24</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3200,22 +3197,22 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to better comply with UiPath standards
Changes applied:

- Updated annotations, activities names, variable names.
- Deleted "GetAppCredentials.xaml" to ensure the SecureString usage compliance
</commit_message>
<xml_diff>
--- a/src/Data/Config.xlsx
+++ b/src/Data/Config.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\nicoerlichman\Documents\2-Code_Repos\UiPath\Custom-REFramework\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C7CBC-A70C-4302-87DE-16F754E93466}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8124F88-01ED-4372-9C51-09B548FB8EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21435" windowHeight="11340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
     <sheet name="Settings" sheetId="1" r:id="rId2"/>
     <sheet name="Credentials" sheetId="6" r:id="rId3"/>
-    <sheet name="Assets" sheetId="4" r:id="rId4"/>
-    <sheet name="Constants" sheetId="2" r:id="rId5"/>
+    <sheet name="Constants" sheetId="2" r:id="rId4"/>
+    <sheet name="Assets" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>MaxRetryNumber</t>
   </si>
@@ -314,6 +314,21 @@
   </si>
   <si>
     <t>Report_DescriptionColumnName</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Description (Assets will always overwrite other config)</t>
   </si>
 </sst>
 </file>
@@ -527,8 +542,8 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -551,9 +566,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Nicolas Erlichman" id="{C9125C45-73CB-4C5F-A17E-BFB4B4F53EE3}" userId="Nicolas Erlichman" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,7 +868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B9EE4A-A787-482A-9A13-E1DF8641FC90}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -972,7 +987,7 @@
   <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1017,25 +1032,40 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="18" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="18" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3040,43 +3070,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="3" max="3" width="75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3341,13 +3340,13 @@
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3363,13 +3362,13 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4341,4 +4340,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>